<commit_message>
update data to numeric
</commit_message>
<xml_diff>
--- a/Objective1CompiledDataWithIndex.xlsx
+++ b/Objective1CompiledDataWithIndex.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthiew\Documents\Research\Objective 1 - Paired Comparisons\StudyAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthiew\Documents\Research\GitHub\Objective1\Objective1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55AD888F-C30B-44B4-8997-D124B3A65287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8D3E43-DE2E-41CF-BC3A-204FA1A786C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" tabRatio="930" xr2:uid="{F48DFC96-7555-4FDB-A91F-73438CE1E98C}"/>
+    <workbookView xWindow="-29355" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="930" firstSheet="4" activeTab="11" xr2:uid="{F48DFC96-7555-4FDB-A91F-73438CE1E98C}"/>
   </bookViews>
   <sheets>
     <sheet name="INDEX" sheetId="13" r:id="rId1"/>
@@ -1378,7 +1378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1401,6 +1401,7 @@
     <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1982,18 +1983,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B2C32-2A2B-4843-95C1-F8AB56B546E7}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.40625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>206</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2014,7 +2015,7 @@
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2027,7 +2028,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2040,7 +2041,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2053,7 +2054,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2066,7 +2067,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2079,7 +2080,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2092,7 +2093,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2105,7 +2106,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2118,7 +2119,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2131,7 +2132,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2144,7 +2145,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2157,7 +2158,7 @@
         <v>Go to Sheet</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2183,12 +2184,12 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>0</v>
@@ -2293,7 +2294,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>31</v>
       </c>
@@ -2400,7 +2401,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2507,7 +2508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -2614,7 +2615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -2721,7 +2722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>35</v>
       </c>
@@ -2828,7 +2829,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2935,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -3042,7 +3043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -3149,7 +3150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>39</v>
       </c>
@@ -3256,7 +3257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -3363,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -3470,7 +3471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>43</v>
       </c>
@@ -3684,7 +3685,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -3791,7 +3792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -3898,7 +3899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -4005,7 +4006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>47</v>
       </c>
@@ -4112,7 +4113,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -4219,7 +4220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -4326,7 +4327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -4433,7 +4434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>51</v>
       </c>
@@ -4540,7 +4541,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -4647,7 +4648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -4754,7 +4755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -4875,12 +4876,12 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>0</v>
@@ -4985,7 +4986,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>119</v>
       </c>
@@ -5092,7 +5093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -5199,7 +5200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -5306,7 +5307,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>179</v>
       </c>
@@ -5413,7 +5414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>120</v>
       </c>
@@ -5520,7 +5521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -5627,7 +5628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>180</v>
       </c>
@@ -5734,7 +5735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>181</v>
       </c>
@@ -5841,7 +5842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>121</v>
       </c>
@@ -5948,7 +5949,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>115</v>
       </c>
@@ -6055,7 +6056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -6162,7 +6163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>183</v>
       </c>
@@ -6269,7 +6270,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>122</v>
       </c>
@@ -6376,7 +6377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -6483,7 +6484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>184</v>
       </c>
@@ -6590,7 +6591,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>185</v>
       </c>
@@ -6697,7 +6698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>123</v>
       </c>
@@ -6804,7 +6805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>117</v>
       </c>
@@ -6911,7 +6912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -7018,7 +7019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>187</v>
       </c>
@@ -7125,7 +7126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>124</v>
       </c>
@@ -7232,7 +7233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -7339,7 +7340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>188</v>
       </c>
@@ -7446,7 +7447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>189</v>
       </c>
@@ -7563,16 +7564,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEFA15DD-6C74-473C-9FB3-70164FB53576}">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="B2:AI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>0</v>
@@ -7677,114 +7678,114 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="20">
         <v>13</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="20">
         <v>13</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="20">
         <v>15</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="20">
         <v>13</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="20">
         <v>13</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="20">
         <v>15</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="20">
         <v>13</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="20">
         <v>15</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="20">
         <v>13</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="20">
         <v>13</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="20">
         <v>13</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="20">
         <v>15</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="20">
         <v>15</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="20">
         <v>15</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="20">
         <v>13</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="20">
         <v>13</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="20">
         <v>15</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="20">
         <v>13</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="20">
         <v>15</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="20">
         <v>13</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="20">
         <v>15</v>
       </c>
-      <c r="W2" s="5">
+      <c r="W2" s="20">
         <v>13</v>
       </c>
-      <c r="X2" s="4">
+      <c r="X2" s="20">
         <v>15</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="Y2" s="20">
         <v>13</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="Z2" s="20">
         <v>13</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AA2" s="20">
         <v>15</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="20">
         <v>13</v>
       </c>
-      <c r="AC2" s="4">
+      <c r="AC2" s="20">
         <v>15</v>
       </c>
-      <c r="AD2" s="4">
+      <c r="AD2" s="20">
         <v>15</v>
       </c>
-      <c r="AE2" s="4">
+      <c r="AE2" s="20">
         <v>15</v>
       </c>
-      <c r="AF2" s="4">
+      <c r="AF2" s="20">
         <v>15</v>
       </c>
-      <c r="AG2" s="4">
+      <c r="AG2" s="20">
         <v>15</v>
       </c>
-      <c r="AH2" s="4">
+      <c r="AH2" s="20">
         <v>15</v>
       </c>
-      <c r="AI2" s="4">
+      <c r="AI2" s="20">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -7891,7 +7892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -7998,7 +7999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -8105,7 +8106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
@@ -8212,7 +8213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -8319,7 +8320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -8426,7 +8427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -8533,7 +8534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>62</v>
       </c>
@@ -8640,7 +8641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -8747,7 +8748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -8854,7 +8855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -8961,7 +8962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>65</v>
       </c>
@@ -9068,7 +9069,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -9175,7 +9176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -9282,7 +9283,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -9389,7 +9390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>68</v>
       </c>
@@ -9496,7 +9497,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -9603,7 +9604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -9710,7 +9711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -9817,7 +9818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>71</v>
       </c>
@@ -9924,7 +9925,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -10031,7 +10032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -10138,7 +10139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -10259,9 +10260,9 @@
       <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -10311,7 +10312,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -10358,7 +10359,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -10405,7 +10406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -10452,7 +10453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -10499,7 +10500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -10546,7 +10547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -10587,7 +10588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -10634,7 +10635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -10681,7 +10682,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -10725,7 +10726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -10772,7 +10773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -10819,7 +10820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -10863,7 +10864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -10907,7 +10908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -10951,7 +10952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -11001,7 +11002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -11042,7 +11043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -11086,7 +11087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -11133,7 +11134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -11180,7 +11181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -11224,7 +11225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -11271,7 +11272,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -11318,7 +11319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -11365,7 +11366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -11412,7 +11413,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -11456,7 +11457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -11500,7 +11501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -11541,7 +11542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -11582,7 +11583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -11623,7 +11624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -11667,7 +11668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -11714,7 +11715,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>94</v>
       </c>
@@ -11758,7 +11759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>176</v>
       </c>
@@ -11805,7 +11806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>177</v>
       </c>
@@ -11863,12 +11864,12 @@
       <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>0</v>
@@ -11961,7 +11962,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -12056,7 +12057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -12151,7 +12152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -12246,7 +12247,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -12341,7 +12342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -12436,7 +12437,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -12531,7 +12532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -12626,7 +12627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -12721,7 +12722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -12816,7 +12817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -12911,7 +12912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -13006,7 +13007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -13101,7 +13102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
@@ -13196,7 +13197,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -13291,7 +13292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -13386,7 +13387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -13481,7 +13482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -13576,7 +13577,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -13671,7 +13672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -13766,7 +13767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -13861,7 +13862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
@@ -13956,7 +13957,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -14051,7 +14052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -14146,7 +14147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -14251,16 +14252,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACBFB94-A141-444E-B6E3-4CC43DE7274B}">
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>0</v>
@@ -14353,7 +14354,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
@@ -14408,7 +14409,7 @@
       <c r="R2" s="4">
         <v>13</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="20">
         <v>15</v>
       </c>
       <c r="T2" s="4">
@@ -14448,7 +14449,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -14543,7 +14544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -14638,7 +14639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -14733,7 +14734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
@@ -14828,7 +14829,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -14923,7 +14924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -15018,7 +15019,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -15113,7 +15114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>62</v>
       </c>
@@ -15208,7 +15209,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -15303,7 +15304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -15398,7 +15399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -15493,7 +15494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>65</v>
       </c>
@@ -15588,7 +15589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -15683,7 +15684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -15778,7 +15779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -15873,7 +15874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>68</v>
       </c>
@@ -15968,7 +15969,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -16063,7 +16064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -16158,7 +16159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -16253,7 +16254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>71</v>
       </c>
@@ -16348,7 +16349,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -16443,7 +16444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -16538,7 +16539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -16647,9 +16648,9 @@
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -16690,7 +16691,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -16731,7 +16732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -16772,7 +16773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -16813,7 +16814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -16854,7 +16855,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -16895,7 +16896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -16936,7 +16937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -16977,7 +16978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -17018,7 +17019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -17059,7 +17060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -17100,7 +17101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -17141,7 +17142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -17182,7 +17183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -17223,7 +17224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -17264,7 +17265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -17305,7 +17306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -17346,7 +17347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -17387,7 +17388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -17428,7 +17429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -17469,7 +17470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -17510,7 +17511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -17551,7 +17552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -17592,7 +17593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -17633,7 +17634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -17674,7 +17675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -17715,7 +17716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -17756,7 +17757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -17797,7 +17798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -17838,7 +17839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -17879,7 +17880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -17934,12 +17935,12 @@
       <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>0</v>
@@ -18038,7 +18039,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>95</v>
       </c>
@@ -18139,7 +18140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -18240,7 +18241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -18341,7 +18342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -18442,7 +18443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>98</v>
       </c>
@@ -18543,7 +18544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -18644,7 +18645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -18745,7 +18746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -18846,7 +18847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>101</v>
       </c>
@@ -18947,7 +18948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>115</v>
       </c>
@@ -19048,7 +19049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -19149,7 +19150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -19250,7 +19251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>104</v>
       </c>
@@ -19351,7 +19352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -19452,7 +19453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -19553,7 +19554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>106</v>
       </c>
@@ -19654,7 +19655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>107</v>
       </c>
@@ -19755,7 +19756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>117</v>
       </c>
@@ -19856,7 +19857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>108</v>
       </c>
@@ -19957,7 +19958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -20058,7 +20059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>110</v>
       </c>
@@ -20159,7 +20160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -20260,7 +20261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -20361,7 +20362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -20476,9 +20477,9 @@
       <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -20528,7 +20529,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -20572,7 +20573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -20619,7 +20620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -20666,7 +20667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -20713,7 +20714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -20760,7 +20761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -20807,7 +20808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -20851,7 +20852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -20898,7 +20899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -20945,7 +20946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -20992,7 +20993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -21039,7 +21040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -21080,7 +21081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -21127,7 +21128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -21171,7 +21172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -21215,7 +21216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -21262,7 +21263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -21309,7 +21310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -21356,7 +21357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -21400,7 +21401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -21447,7 +21448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -21491,7 +21492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -21538,7 +21539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -21585,7 +21586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -21632,7 +21633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -21679,7 +21680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -21726,7 +21727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -21767,7 +21768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -21811,7 +21812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -21858,7 +21859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -21905,7 +21906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -21952,7 +21953,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>94</v>
       </c>
@@ -22012,12 +22013,12 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>0</v>
@@ -22110,7 +22111,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>119</v>
       </c>
@@ -22205,7 +22206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -22300,7 +22301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>209</v>
       </c>
@@ -22395,7 +22396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>210</v>
       </c>
@@ -22490,7 +22491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>120</v>
       </c>
@@ -22585,7 +22586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -22680,7 +22681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>211</v>
       </c>
@@ -22775,7 +22776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>212</v>
       </c>
@@ -22870,7 +22871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>121</v>
       </c>
@@ -22965,7 +22966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>115</v>
       </c>
@@ -23060,7 +23061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -23155,7 +23156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>214</v>
       </c>
@@ -23250,7 +23251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>122</v>
       </c>
@@ -23345,7 +23346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -23440,7 +23441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>215</v>
       </c>
@@ -23535,7 +23536,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>216</v>
       </c>
@@ -23630,7 +23631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>123</v>
       </c>
@@ -23725,7 +23726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>117</v>
       </c>
@@ -23820,7 +23821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>217</v>
       </c>
@@ -23915,7 +23916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>218</v>
       </c>
@@ -24010,7 +24011,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>124</v>
       </c>
@@ -24105,7 +24106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -24200,7 +24201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>219</v>
       </c>
@@ -24295,7 +24296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>220</v>
       </c>
@@ -24404,9 +24405,9 @@
       <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -24456,7 +24457,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -24503,7 +24504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -24547,7 +24548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -24594,7 +24595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -24638,7 +24639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -24682,7 +24683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -24729,7 +24730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -24776,7 +24777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -24820,7 +24821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -24867,7 +24868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -24914,7 +24915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -24961,7 +24962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -25005,7 +25006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -25049,7 +25050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -25096,7 +25097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -25137,7 +25138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -25181,7 +25182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -25228,7 +25229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -25275,7 +25276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -25316,7 +25317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -25360,7 +25361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -25407,7 +25408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -25454,7 +25455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -25501,7 +25502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -25542,7 +25543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -25583,7 +25584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -25630,7 +25631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -25674,7 +25675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -25721,7 +25722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -25765,7 +25766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -25826,12 +25827,12 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>0</v>
@@ -25936,7 +25937,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>95</v>
       </c>
@@ -26043,7 +26044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -26150,7 +26151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -26257,7 +26258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -26364,7 +26365,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>98</v>
       </c>
@@ -26471,7 +26472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -26578,7 +26579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -26685,7 +26686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -26792,7 +26793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>101</v>
       </c>
@@ -26899,7 +26900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>115</v>
       </c>
@@ -27006,7 +27007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -27113,7 +27114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -27220,7 +27221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>104</v>
       </c>
@@ -27327,7 +27328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -27434,7 +27435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -27541,7 +27542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>106</v>
       </c>
@@ -27648,7 +27649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>107</v>
       </c>
@@ -27755,7 +27756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>117</v>
       </c>
@@ -27862,7 +27863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>108</v>
       </c>
@@ -27969,7 +27970,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -28076,7 +28077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>110</v>
       </c>
@@ -28183,7 +28184,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -28290,7 +28291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -28397,7 +28398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>112</v>
       </c>

</xml_diff>